<commit_message>
update combined runtime '
</commit_message>
<xml_diff>
--- a/2022_FFT_benchmarks.xlsx
+++ b/2022_FFT_benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmyliu/Documents/University/2021/INFO4001/git_repo/Jimmy-nonImageData-Image/Jimmy-NonImgToImg-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3EAB14-4806-7A43-BF99-3D4BEDFBE9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061FE978-CC43-D54B-A94A-835CFED8FA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="500" windowWidth="27860" windowHeight="17500" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,12 +138,6 @@
     <t>Combined</t>
   </si>
   <si>
-    <t>11min40s</t>
-  </si>
-  <si>
-    <t>18min29s</t>
-  </si>
-  <si>
     <t>CPU Time</t>
   </si>
   <si>
@@ -330,13 +324,19 @@
     <t>MemUsed</t>
   </si>
   <si>
-    <t>5518.27MiB</t>
-  </si>
-  <si>
-    <t>5546.27 MiB</t>
-  </si>
-  <si>
     <t>RAW</t>
+  </si>
+  <si>
+    <t>20min 3s</t>
+  </si>
+  <si>
+    <t>5551.54 MiB</t>
+  </si>
+  <si>
+    <t>9min 11s</t>
+  </si>
+  <si>
+    <t>5518.27 MiB</t>
   </si>
 </sst>
 </file>
@@ -357,10 +357,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -686,10 +688,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -727,10 +729,10 @@
         <v>0.94330000000000003</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -768,10 +770,10 @@
         <v>0.96089999999999998</v>
       </c>
       <c r="L3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -809,10 +811,10 @@
         <v>0.93989999999999996</v>
       </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -1165,10 +1167,10 @@
         <v>0.92549999999999999</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -1206,10 +1208,10 @@
         <v>0.96299999999999997</v>
       </c>
       <c r="L15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -1247,10 +1249,10 @@
         <v>0.92530000000000001</v>
       </c>
       <c r="L16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1306,10 +1308,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -1347,10 +1349,10 @@
         <v>0.94799999999999995</v>
       </c>
       <c r="L2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -1388,10 +1390,10 @@
         <v>0.96020000000000005</v>
       </c>
       <c r="L3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -1429,10 +1431,10 @@
         <v>0.92200000000000004</v>
       </c>
       <c r="L4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -1785,10 +1787,10 @@
         <v>0.81630000000000003</v>
       </c>
       <c r="L14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -1826,10 +1828,10 @@
         <v>0.9325</v>
       </c>
       <c r="L15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -1867,10 +1869,10 @@
         <v>0.91790000000000005</v>
       </c>
       <c r="L16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1926,10 +1928,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -1967,10 +1969,10 @@
         <v>0.97619999999999996</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -2008,10 +2010,10 @@
         <v>0.86129999999999995</v>
       </c>
       <c r="L3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -2049,10 +2051,10 @@
         <v>0.90339999999999998</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -2405,10 +2407,10 @@
         <v>0.95109999999999995</v>
       </c>
       <c r="L14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -2446,10 +2448,10 @@
         <v>0.95279999999999998</v>
       </c>
       <c r="L15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -2487,10 +2489,10 @@
         <v>0.90390000000000004</v>
       </c>
       <c r="L16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2546,10 +2548,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -2587,10 +2589,10 @@
         <v>0.88580000000000003</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -2628,10 +2630,10 @@
         <v>0.87409999999999999</v>
       </c>
       <c r="L3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -2669,10 +2671,10 @@
         <v>0.85419999999999996</v>
       </c>
       <c r="L4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -3025,10 +3027,10 @@
         <v>0.90149999999999997</v>
       </c>
       <c r="L14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -3066,10 +3068,10 @@
         <v>0.74880000000000002</v>
       </c>
       <c r="L15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -3107,10 +3109,10 @@
         <v>0.86350000000000005</v>
       </c>
       <c r="L16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -3167,10 +3169,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -3208,10 +3210,10 @@
         <v>0.92390000000000005</v>
       </c>
       <c r="L2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -3249,10 +3251,10 @@
         <v>0.92130000000000001</v>
       </c>
       <c r="L3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -3290,10 +3292,10 @@
         <v>0.90349999999999997</v>
       </c>
       <c r="L4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -3646,10 +3648,10 @@
         <v>0.94059999999999999</v>
       </c>
       <c r="L14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -3687,10 +3689,10 @@
         <v>0.95489999999999997</v>
       </c>
       <c r="L15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -3728,10 +3730,10 @@
         <v>0.93969999999999998</v>
       </c>
       <c r="L16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -3787,10 +3789,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -3828,10 +3830,10 @@
         <v>0.48609999999999998</v>
       </c>
       <c r="L2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -3869,10 +3871,10 @@
         <v>0.43330000000000002</v>
       </c>
       <c r="L3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -3910,10 +3912,10 @@
         <v>0.40339999999999998</v>
       </c>
       <c r="L4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -4266,10 +4268,10 @@
         <v>0.4667</v>
       </c>
       <c r="L14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -4307,10 +4309,10 @@
         <v>0.50870000000000004</v>
       </c>
       <c r="L15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -4348,10 +4350,10 @@
         <v>0.38119999999999998</v>
       </c>
       <c r="L16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -4364,7 +4366,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4404,10 +4406,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -4445,10 +4447,10 @@
         <v>0.83409999999999995</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="M2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -4486,10 +4488,10 @@
         <v>0.83260000000000001</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="M3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -4512,7 +4514,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H4" s="10">
         <v>0.72670000000000001</v>
@@ -4548,7 +4550,7 @@
         <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H5" s="10">
         <v>0.67420000000000002</v>
@@ -4584,7 +4586,7 @@
         <v>17</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H6" s="10">
         <v>0.32129999999999997</v>
@@ -4658,10 +4660,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -4699,10 +4701,10 @@
         <v>0.97650000000000003</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -4740,10 +4742,10 @@
         <v>0.9839</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -4781,10 +4783,10 @@
         <v>0.97350000000000003</v>
       </c>
       <c r="L4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -5137,10 +5139,10 @@
         <v>0.98450000000000004</v>
       </c>
       <c r="L14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -5178,10 +5180,10 @@
         <v>0.99209999999999998</v>
       </c>
       <c r="L15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -5219,10 +5221,10 @@
         <v>0.97440000000000004</v>
       </c>
       <c r="L16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -5278,10 +5280,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -5319,10 +5321,10 @@
         <v>0.99070000000000003</v>
       </c>
       <c r="L2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -5360,10 +5362,10 @@
         <v>0.99460000000000004</v>
       </c>
       <c r="L3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -5401,10 +5403,10 @@
         <v>0.9869</v>
       </c>
       <c r="L4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -5757,10 +5759,10 @@
         <v>0.96879999999999999</v>
       </c>
       <c r="L14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -5798,10 +5800,10 @@
         <v>0.98399999999999999</v>
       </c>
       <c r="L15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -5839,10 +5841,10 @@
         <v>0.96850000000000003</v>
       </c>
       <c r="L16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -5898,10 +5900,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -5939,10 +5941,10 @@
         <v>0.91879999999999995</v>
       </c>
       <c r="L2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -5980,10 +5982,10 @@
         <v>0.94569999999999999</v>
       </c>
       <c r="L3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -6021,10 +6023,10 @@
         <v>0.94030000000000002</v>
       </c>
       <c r="L4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -6377,10 +6379,10 @@
         <v>0.92030000000000001</v>
       </c>
       <c r="L14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -6418,10 +6420,10 @@
         <v>0.96120000000000005</v>
       </c>
       <c r="L15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -6459,10 +6461,10 @@
         <v>0.94359999999999999</v>
       </c>
       <c r="L16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -6518,10 +6520,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15">
@@ -6559,10 +6561,10 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15">
@@ -6600,10 +6602,10 @@
         <v>0.94199999999999995</v>
       </c>
       <c r="L3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15">
@@ -6641,10 +6643,10 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15">
@@ -6997,10 +6999,10 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -7038,10 +7040,10 @@
         <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -7079,10 +7081,10 @@
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -7138,10 +7140,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -7179,10 +7181,10 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -7220,10 +7222,10 @@
         <v>0.99539999999999995</v>
       </c>
       <c r="L3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -7261,10 +7263,10 @@
         <v>0.98870000000000002</v>
       </c>
       <c r="L4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -7617,10 +7619,10 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -7658,10 +7660,10 @@
         <v>0.99480000000000002</v>
       </c>
       <c r="L15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -7699,10 +7701,10 @@
         <v>0.97099999999999997</v>
       </c>
       <c r="L16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -7758,10 +7760,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -7799,10 +7801,10 @@
         <v>0.6492</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -7840,10 +7842,10 @@
         <v>0.59519999999999995</v>
       </c>
       <c r="L3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -7881,10 +7883,10 @@
         <v>0.65780000000000005</v>
       </c>
       <c r="L4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -8237,10 +8239,10 @@
         <v>0.52980000000000005</v>
       </c>
       <c r="L14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -8278,10 +8280,10 @@
         <v>0.4738</v>
       </c>
       <c r="L15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -8319,10 +8321,10 @@
         <v>0.5262</v>
       </c>
       <c r="L16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -8379,10 +8381,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -8420,10 +8422,10 @@
         <v>0.98870000000000002</v>
       </c>
       <c r="L2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -8461,10 +8463,10 @@
         <v>0.98250000000000004</v>
       </c>
       <c r="L3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -8502,10 +8504,10 @@
         <v>0.96489999999999998</v>
       </c>
       <c r="L4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -8858,10 +8860,10 @@
         <v>0.95760000000000001</v>
       </c>
       <c r="L14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -8899,10 +8901,10 @@
         <v>0.98370000000000002</v>
       </c>
       <c r="L15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -8940,10 +8942,10 @@
         <v>0.96760000000000002</v>
       </c>
       <c r="L16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -8999,10 +9001,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -9040,10 +9042,10 @@
         <v>0.80810000000000004</v>
       </c>
       <c r="L2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
@@ -9081,10 +9083,10 @@
         <v>0.3261</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
@@ -9122,10 +9124,10 @@
         <v>0.69310000000000005</v>
       </c>
       <c r="L4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
@@ -9478,10 +9480,10 @@
         <v>0.9153</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
@@ -9519,10 +9521,10 @@
         <v>0.11990000000000001</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
@@ -9560,10 +9562,10 @@
         <v>0.79049999999999998</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>